<commit_message>
add sign and date
</commit_message>
<xml_diff>
--- a/modelo certificado.xlsx
+++ b/modelo certificado.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SPIDER-DEV\UAI\emitir_certificados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC - CAROLINE\Videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A24E17-C579-43AA-B65D-6B8E0408B337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46536BC0-7DC2-464E-A77D-E77081D91620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="311" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4170" windowWidth="29040" windowHeight="15840" tabRatio="311" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CARA" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="177">
+  <si>
+    <t>CIENCIAS DE LA SALUD</t>
+  </si>
+  <si>
+    <t>ENFERMERÍA</t>
+  </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -47,18 +53,291 @@
     <t>PRIMER CICLO</t>
   </si>
   <si>
+    <t>10A01</t>
+  </si>
+  <si>
+    <t>Matemática I</t>
+  </si>
+  <si>
+    <t>R.D Nº233-2024-FCS</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>10A02</t>
+  </si>
+  <si>
+    <t>Pensamiento Crítico</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>10A03</t>
+  </si>
+  <si>
+    <t>Filosofía y Ética</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>10A04</t>
+  </si>
+  <si>
+    <t>Taller de Comunicación Oral</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>10A05</t>
+  </si>
+  <si>
+    <t>Globalización y Realidad Nacional</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>10A06</t>
+  </si>
+  <si>
+    <t>Cultura Ambiental</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
     <t>SEGUNDO CICLO</t>
   </si>
   <si>
+    <t>10A07</t>
+  </si>
+  <si>
+    <t>Matemática II</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>10A08</t>
+  </si>
+  <si>
+    <t>Metodología de Investigación</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>10A09</t>
+  </si>
+  <si>
+    <t>Emprendimiento</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>10A10</t>
+  </si>
+  <si>
+    <t>Taller de Comunicación Escrita</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>10A11</t>
+  </si>
+  <si>
+    <t>Administración  General</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>21A01</t>
+  </si>
+  <si>
+    <t>Actividades de Proyección Social I</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
     <t>TERCER CICLO</t>
   </si>
   <si>
+    <t>21A02</t>
+  </si>
+  <si>
+    <t>Anatomía y  Fisiología</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>21A03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estadística </t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>21A04</t>
+  </si>
+  <si>
+    <t>Biología</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>21A05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Métodos de Atención en Enfermería </t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>21A06</t>
+  </si>
+  <si>
+    <t>Antropología de la Salud</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>21A07</t>
+  </si>
+  <si>
+    <t>Actividades de Proyección Social II</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
     <t>CUARTO CICLO</t>
   </si>
   <si>
+    <t>21A08</t>
+  </si>
+  <si>
+    <t>Semiología</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>21A09</t>
+  </si>
+  <si>
+    <t>Química y Bioquímica</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>21A10</t>
+  </si>
+  <si>
+    <t>Microbiología y Parasitología</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>21A11</t>
+  </si>
+  <si>
+    <t>Enfermería Clínica</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>21A12</t>
+  </si>
+  <si>
+    <t>Enfermería Pediatríca</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>21A13</t>
+  </si>
+  <si>
+    <t>Actividades de Proyección Social III</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
     <t>QUINTO CICLO</t>
   </si>
   <si>
+    <t>21A14</t>
+  </si>
+  <si>
+    <t>Farmacología y Terapeutica</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>21A15</t>
+  </si>
+  <si>
+    <t>Enfermería en Atención Primaria de Salud I</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>21A16</t>
+  </si>
+  <si>
+    <t>Enfermería en Salud Comunitaria I</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>21A17</t>
+  </si>
+  <si>
+    <t>Nutrición y Dietoterapia</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>21A18</t>
+  </si>
+  <si>
+    <t>Enfermería en Salud del Adulto I</t>
+  </si>
+  <si>
+    <t>029</t>
+  </si>
+  <si>
+    <t>21A19</t>
+  </si>
+  <si>
+    <t>Actividades de Proyección Social IV</t>
+  </si>
+  <si>
+    <t>030</t>
+  </si>
+  <si>
     <t>21AA1</t>
   </si>
   <si>
@@ -80,6 +359,15 @@
     <t>050</t>
   </si>
   <si>
+    <t>21A20</t>
+  </si>
+  <si>
+    <t>Salud Pública y Epidemiología</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
     <t>21AA3</t>
   </si>
   <si>
@@ -89,6 +377,15 @@
     <t>051</t>
   </si>
   <si>
+    <t>21A21</t>
+  </si>
+  <si>
+    <t>Enfermería en Atención Primaria de Salud II</t>
+  </si>
+  <si>
+    <t>032</t>
+  </si>
+  <si>
     <t>21AA4</t>
   </si>
   <si>
@@ -98,6 +395,15 @@
     <t>052</t>
   </si>
   <si>
+    <t>21A22</t>
+  </si>
+  <si>
+    <t>Enfermería Geriátrica</t>
+  </si>
+  <si>
+    <t>033</t>
+  </si>
+  <si>
     <t>21AA5</t>
   </si>
   <si>
@@ -107,6 +413,15 @@
     <t>053</t>
   </si>
   <si>
+    <t>21A23</t>
+  </si>
+  <si>
+    <t>Enfermería en Medicina Alternativa</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
     <t>21AA6</t>
   </si>
   <si>
@@ -116,16 +431,145 @@
     <t>054</t>
   </si>
   <si>
+    <t>21A24</t>
+  </si>
+  <si>
+    <t>Enfermería en Salud del Adulto II</t>
+  </si>
+  <si>
+    <t>035</t>
+  </si>
+  <si>
     <t>SEPTIMO CICLO</t>
   </si>
   <si>
+    <t>21A25</t>
+  </si>
+  <si>
+    <t>Taller de Investigación I</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>21A26</t>
+  </si>
+  <si>
+    <t>Enfermería en Emergencias y Desastres</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>21A27</t>
+  </si>
+  <si>
+    <t>Enfermería en Salud Mental y Psiquiatría</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>21A28</t>
+  </si>
+  <si>
+    <t>Enfermería en Salud de la Mujer</t>
+  </si>
+  <si>
+    <t>039</t>
+  </si>
+  <si>
+    <t>21A29</t>
+  </si>
+  <si>
+    <t>Inglés I</t>
+  </si>
+  <si>
+    <t>040</t>
+  </si>
+  <si>
     <t>OCTAVO CICLO</t>
   </si>
   <si>
+    <t>21A30</t>
+  </si>
+  <si>
+    <t>Enfermería en Salud Comunitaria II</t>
+  </si>
+  <si>
+    <t>041</t>
+  </si>
+  <si>
+    <t>21A31</t>
+  </si>
+  <si>
+    <t>Taller de Investigación II</t>
+  </si>
+  <si>
+    <t>042</t>
+  </si>
+  <si>
+    <t>21A32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internado I </t>
+  </si>
+  <si>
+    <t>043</t>
+  </si>
+  <si>
+    <t>21A33</t>
+  </si>
+  <si>
+    <t>Inglés II</t>
+  </si>
+  <si>
+    <t>044</t>
+  </si>
+  <si>
     <t>NOVENO CICLO</t>
   </si>
   <si>
+    <t>045</t>
+  </si>
+  <si>
+    <t>21A35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internado II </t>
+  </si>
+  <si>
+    <t>046</t>
+  </si>
+  <si>
     <t>DECIMO CICLO</t>
+  </si>
+  <si>
+    <t>047</t>
+  </si>
+  <si>
+    <t>21A37</t>
+  </si>
+  <si>
+    <t>Internado III</t>
+  </si>
+  <si>
+    <t>048</t>
+  </si>
+  <si>
+    <t>Seminario de Tesis</t>
+  </si>
+  <si>
+    <t>P02X2151</t>
+  </si>
+  <si>
+    <t>P02X2153</t>
+  </si>
+  <si>
+    <t>Trabajo de Investigación</t>
+  </si>
+  <si>
+    <t>TORRES CARBAJAL , FELICITA NICOLE</t>
   </si>
 </sst>
 </file>
@@ -309,7 +753,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -407,6 +851,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -416,6 +863,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -480,38 +928,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Moneda 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1457,11 +1873,11 @@
   </sheetPr>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:I7"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="13" customWidth="1"/>
@@ -1483,23 +1899,27 @@
     <row r="2" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:16" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="46"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
     </row>
     <row r="5" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="38"/>
+      <c r="D5" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="49">
+        <v>74500285</v>
+      </c>
+      <c r="J5" s="40"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="6"/>
@@ -1507,13 +1927,15 @@
     <row r="6" spans="1:16" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="38"/>
+      <c r="D6" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="40"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="6"/>
@@ -1521,44 +1943,46 @@
     <row r="7" spans="1:16" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="38"/>
+      <c r="D7" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="40"/>
       <c r="L7" s="14"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="38"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="9" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="47"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="49"/>
     </row>
     <row r="10" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="47"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="46"/>
+      <c r="I10" s="49"/>
     </row>
     <row r="11" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
@@ -1590,137 +2014,252 @@
     <row r="13" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
+        <v>3</v>
+      </c>
+      <c r="C13" s="40"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="38" t="str">
+      <c r="I13" s="40" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J13" s="19"/>
       <c r="M13" s="8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="38"/>
+      <c r="F14" s="57">
+        <v>16</v>
+      </c>
+      <c r="G14" s="4" t="str">
+        <f>IF(F14=11,"ONCE",IF(F14=12,"DOCE",IF(F14=13,"TRECE",IF(F14=14,"CATORCE",IF(F14=15,"QUINCE",IF(F14=16,"DIECISEIS",IF(F14=17,"DIECISIETE",IF(F14=18,"DIECIOCHO", IF(F14=19,"DIECINUEVE",IF(F14=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISEIS</v>
+      </c>
+      <c r="H14" s="4">
+        <v>4</v>
+      </c>
+      <c r="I14" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J14" s="19"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="11"/>
+      <c r="N14" s="43">
+        <v>20202</v>
+      </c>
+      <c r="O14" s="4">
+        <v>21</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="38"/>
+      <c r="F15" s="57">
+        <v>15</v>
+      </c>
+      <c r="G15" s="4" t="str">
+        <f>IF(F15=11,"ONCE",IF(F15=12,"DOCE",IF(F15=13,"TRECE",IF(F15=14,"CATORCE",IF(F15=15,"QUINCE",IF(F15=16,"DIECISEIS",IF(F15=17,"DIECISIETE",IF(F15=18,"DIECIOCHO", IF(F15=19,"DIECINUEVE",IF(F15=20,"VEINTE",ERROR))))))))))</f>
+        <v>QUINCE</v>
+      </c>
+      <c r="H15" s="4">
+        <v>4</v>
+      </c>
+      <c r="I15" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J15" s="19"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="11"/>
+      <c r="N15" s="43">
+        <v>20202</v>
+      </c>
+      <c r="O15" s="4">
+        <v>21</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="38"/>
+      <c r="F16" s="57">
+        <v>17</v>
+      </c>
+      <c r="G16" s="4" t="str">
+        <f>IF(F16=11,"ONCE",IF(F16=12,"DOCE",IF(F16=13,"TRECE",IF(F16=14,"CATORCE",IF(F16=15,"QUINCE",IF(F16=16,"DIECISEIS",IF(F16=17,"DIECISIETE",IF(F16=18,"DIECIOCHO", IF(F16=19,"DIECINUEVE",IF(F16=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="H16" s="4">
+        <v>3</v>
+      </c>
+      <c r="I16" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J16" s="19"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="11"/>
+      <c r="N16" s="43">
+        <v>20202</v>
+      </c>
+      <c r="O16" s="4">
+        <v>21</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="E17" s="9"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="38"/>
+      <c r="F17" s="57">
+        <v>14</v>
+      </c>
+      <c r="G17" s="4" t="str">
+        <f>IF(F17=11,"ONCE",IF(F17=12,"DOCE",IF(F17=13,"TRECE",IF(F17=14,"CATORCE",IF(F17=15,"QUINCE",IF(F17=16,"DIECISEIS",IF(F17=17,"DIECISIETE",IF(F17=18,"DIECIOCHO", IF(F17=19,"DIECINUEVE",IF(F17=20,"VEINTE",ERROR))))))))))</f>
+        <v>CATORCE</v>
+      </c>
+      <c r="H17" s="4">
+        <v>4</v>
+      </c>
+      <c r="I17" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J17" s="19"/>
       <c r="M17" s="9"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="11"/>
+      <c r="N17" s="43">
+        <v>20202</v>
+      </c>
+      <c r="O17" s="4">
+        <v>21</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="E18" s="9"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="38"/>
+      <c r="F18" s="57">
+        <v>16</v>
+      </c>
+      <c r="G18" s="4" t="str">
+        <f>IF(F18=11,"ONCE",IF(F18=12,"DOCE",IF(F18=13,"TRECE",IF(F18=14,"CATORCE",IF(F18=15,"QUINCE",IF(F18=16,"DIECISEIS",IF(F18=17,"DIECISIETE",IF(F18=18,"DIECIOCHO", IF(F18=19,"DIECINUEVE",IF(F18=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISEIS</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3</v>
+      </c>
+      <c r="I18" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J18" s="19"/>
       <c r="M18" s="9"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="11"/>
+      <c r="N18" s="43">
+        <v>20202</v>
+      </c>
+      <c r="O18" s="4">
+        <v>21</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="E19" s="9"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="38"/>
+      <c r="F19" s="57">
+        <v>12</v>
+      </c>
+      <c r="G19" s="4" t="str">
+        <f>IF(F19=11,"ONCE",IF(F19=12,"DOCE",IF(F19=13,"TRECE",IF(F19=14,"CATORCE",IF(F19=15,"QUINCE",IF(F19=16,"DIECISEIS",IF(F19=17,"DIECISIETE",IF(F19=18,"DIECIOCHO", IF(F19=19,"DIECINUEVE",IF(F19=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="H19" s="4">
+        <v>3</v>
+      </c>
+      <c r="I19" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>2021121006</v>
+      </c>
       <c r="J19" s="19"/>
       <c r="M19" s="9"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="11"/>
+      <c r="N19" s="43">
+        <v>20211</v>
+      </c>
+      <c r="O19" s="4">
+        <v>21</v>
+      </c>
+      <c r="P19" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
+        <v>23</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="38" t="str">
+      <c r="I20" s="40" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J20" s="19"/>
       <c r="M20" s="8" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="N20" s="19"/>
       <c r="O20" s="4"/>
@@ -1728,233 +2267,461 @@
     </row>
     <row r="21" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="E21" s="9"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="38"/>
+      <c r="F21" s="57">
+        <v>11</v>
+      </c>
+      <c r="G21" s="4" t="str">
+        <f>IF(F21=11,"ONCE",IF(F21=12,"DOCE",IF(F21=13,"TRECE",IF(F21=14,"CATORCE",IF(F21=15,"QUINCE",IF(F21=16,"DIECISEIS",IF(F21=17,"DIECISIETE",IF(F21=18,"DIECIOCHO", IF(F21=19,"DIECINUEVE",IF(F21=20,"VEINTE",ERROR))))))))))</f>
+        <v>ONCE</v>
+      </c>
+      <c r="H21" s="4">
+        <v>4</v>
+      </c>
+      <c r="I21" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J21" s="19"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="11"/>
+      <c r="N21" s="43">
+        <v>20162</v>
+      </c>
+      <c r="O21" s="4">
+        <v>21</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="E22" s="9"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="38"/>
+      <c r="F22" s="57">
+        <v>11</v>
+      </c>
+      <c r="G22" s="4" t="str">
+        <f>IF(F22=11,"ONCE",IF(F22=12,"DOCE",IF(F22=13,"TRECE",IF(F22=14,"CATORCE",IF(F22=15,"QUINCE",IF(F22=16,"DIECISEIS",IF(F22=17,"DIECISIETE",IF(F22=18,"DIECIOCHO", IF(F22=19,"DIECINUEVE",IF(F22=20,"VEINTE",ERROR))))))))))</f>
+        <v>ONCE</v>
+      </c>
+      <c r="H22" s="4">
+        <v>4</v>
+      </c>
+      <c r="I22" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J22" s="19"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="11"/>
+      <c r="N22" s="43">
+        <v>20162</v>
+      </c>
+      <c r="O22" s="4">
+        <v>21</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="E23" s="9"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="38"/>
+      <c r="F23" s="57">
+        <v>15</v>
+      </c>
+      <c r="G23" s="4" t="str">
+        <f>IF(F23=11,"ONCE",IF(F23=12,"DOCE",IF(F23=13,"TRECE",IF(F23=14,"CATORCE",IF(F23=15,"QUINCE",IF(F23=16,"DIECISEIS",IF(F23=17,"DIECISIETE",IF(F23=18,"DIECIOCHO", IF(F23=19,"DIECINUEVE",IF(F23=20,"VEINTE",ERROR))))))))))</f>
+        <v>QUINCE</v>
+      </c>
+      <c r="H23" s="4">
+        <v>3</v>
+      </c>
+      <c r="I23" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J23" s="19"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="11"/>
+      <c r="N23" s="43">
+        <v>20162</v>
+      </c>
+      <c r="O23" s="4">
+        <v>21</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="24" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="E24" s="9"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="38"/>
+      <c r="F24" s="57">
+        <v>12</v>
+      </c>
+      <c r="G24" s="4" t="str">
+        <f>IF(F24=11,"ONCE",IF(F24=12,"DOCE",IF(F24=13,"TRECE",IF(F24=14,"CATORCE",IF(F24=15,"QUINCE",IF(F24=16,"DIECISEIS",IF(F24=17,"DIECISIETE",IF(F24=18,"DIECIOCHO", IF(F24=19,"DIECINUEVE",IF(F24=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="H24" s="4">
+        <v>4</v>
+      </c>
+      <c r="I24" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J24" s="19"/>
       <c r="M24" s="9"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="11"/>
+      <c r="N24" s="43">
+        <v>20162</v>
+      </c>
+      <c r="O24" s="4">
+        <v>21</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="25" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="E25" s="9"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="38"/>
+      <c r="F25" s="57">
+        <v>12</v>
+      </c>
+      <c r="G25" s="4" t="str">
+        <f>IF(F25=11,"ONCE",IF(F25=12,"DOCE",IF(F25=13,"TRECE",IF(F25=14,"CATORCE",IF(F25=15,"QUINCE",IF(F25=16,"DIECISEIS",IF(F25=17,"DIECISIETE",IF(F25=18,"DIECIOCHO", IF(F25=19,"DIECINUEVE",IF(F25=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="H25" s="4">
+        <v>3</v>
+      </c>
+      <c r="I25" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J25" s="19"/>
       <c r="M25" s="9"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="11"/>
+      <c r="N25" s="43">
+        <v>20162</v>
+      </c>
+      <c r="O25" s="4">
+        <v>21</v>
+      </c>
+      <c r="P25" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="26" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="E26" s="9"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="38"/>
+      <c r="F26" s="57">
+        <v>17</v>
+      </c>
+      <c r="G26" s="4" t="str">
+        <f>IF(F26=11,"ONCE",IF(F26=12,"DOCE",IF(F26=13,"TRECE",IF(F26=14,"CATORCE",IF(F26=15,"QUINCE",IF(F26=16,"DIECISEIS",IF(F26=17,"DIECISIETE",IF(F26=18,"DIECIOCHO", IF(F26=19,"DIECINUEVE",IF(F26=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="H26" s="4">
+        <v>3</v>
+      </c>
+      <c r="I26" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J26" s="19"/>
       <c r="M26" s="9"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="11"/>
+      <c r="N26" s="43">
+        <v>20161</v>
+      </c>
+      <c r="O26" s="4">
+        <v>21</v>
+      </c>
+      <c r="P26" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="27" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
+        <v>42</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="38"/>
+      <c r="I27" s="40"/>
       <c r="J27" s="19"/>
       <c r="M27" s="5" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="N27" s="19"/>
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="E28" s="9"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="38"/>
+      <c r="F28" s="57">
+        <v>14</v>
+      </c>
+      <c r="G28" s="4" t="str">
+        <f>IF(F28=11,"ONCE",IF(F28=12,"DOCE",IF(F28=13,"TRECE",IF(F28=14,"CATORCE",IF(F28=15,"QUINCE",IF(F28=16,"DIECISEIS",IF(F28=17,"DIECISIETE",IF(F28=18,"DIECIOCHO", IF(F28=19,"DIECINUEVE",IF(F28=20,"VEINTE",ERROR))))))))))</f>
+        <v>CATORCE</v>
+      </c>
+      <c r="H28" s="4">
+        <v>4</v>
+      </c>
+      <c r="I28" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J28" s="19"/>
       <c r="M28" s="9"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="11"/>
+      <c r="N28" s="43">
+        <v>20171</v>
+      </c>
+      <c r="O28" s="4">
+        <v>21</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="29" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
-      <c r="B29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="9"/>
+      <c r="D29" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="E29" s="9"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="38"/>
+      <c r="F29" s="57">
+        <v>11</v>
+      </c>
+      <c r="G29" s="4" t="str">
+        <f>IF(F29=11,"ONCE",IF(F29=12,"DOCE",IF(F29=13,"TRECE",IF(F29=14,"CATORCE",IF(F29=15,"QUINCE",IF(F29=16,"DIECISEIS",IF(F29=17,"DIECISIETE",IF(F29=18,"DIECIOCHO", IF(F29=19,"DIECINUEVE",IF(F29=20,"VEINTE",ERROR))))))))))</f>
+        <v>ONCE</v>
+      </c>
+      <c r="H29" s="4">
+        <v>3</v>
+      </c>
+      <c r="I29" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J29" s="19"/>
       <c r="M29" s="9"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="11"/>
+      <c r="N29" s="43">
+        <v>20171</v>
+      </c>
+      <c r="O29" s="4">
+        <v>21</v>
+      </c>
+      <c r="P29" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
-      <c r="B30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="9"/>
+      <c r="D30" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="E30" s="9"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="38"/>
+      <c r="F30" s="57">
+        <v>14</v>
+      </c>
+      <c r="G30" s="4" t="str">
+        <f>IF(F30=11,"ONCE",IF(F30=12,"DOCE",IF(F30=13,"TRECE",IF(F30=14,"CATORCE",IF(F30=15,"QUINCE",IF(F30=16,"DIECISEIS",IF(F30=17,"DIECISIETE",IF(F30=18,"DIECIOCHO", IF(F30=19,"DIECINUEVE",IF(F30=20,"VEINTE",ERROR))))))))))</f>
+        <v>CATORCE</v>
+      </c>
+      <c r="H30" s="4">
+        <v>3</v>
+      </c>
+      <c r="I30" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J30" s="19"/>
       <c r="M30" s="9"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="11"/>
+      <c r="N30" s="43">
+        <v>20171</v>
+      </c>
+      <c r="O30" s="4">
+        <v>21</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="31" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
-      <c r="B31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="9"/>
+      <c r="D31" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="E31" s="9"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="38"/>
+      <c r="F31" s="57">
+        <v>12</v>
+      </c>
+      <c r="G31" s="4" t="str">
+        <f>IF(F31=11,"ONCE",IF(F31=12,"DOCE",IF(F31=13,"TRECE",IF(F31=14,"CATORCE",IF(F31=15,"QUINCE",IF(F31=16,"DIECISEIS",IF(F31=17,"DIECISIETE",IF(F31=18,"DIECIOCHO", IF(F31=19,"DIECINUEVE",IF(F31=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="H31" s="4">
+        <v>4</v>
+      </c>
+      <c r="I31" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J31" s="19"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="41"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="11"/>
+      <c r="N31" s="43">
+        <v>20171</v>
+      </c>
+      <c r="O31" s="4">
+        <v>21</v>
+      </c>
+      <c r="P31" s="11" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="32" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
-      <c r="B32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="9"/>
+      <c r="D32" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="E32" s="9"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="38"/>
+      <c r="F32" s="57">
+        <v>11</v>
+      </c>
+      <c r="G32" s="4" t="str">
+        <f>IF(F32=11,"ONCE",IF(F32=12,"DOCE",IF(F32=13,"TRECE",IF(F32=14,"CATORCE",IF(F32=15,"QUINCE",IF(F32=16,"DIECISEIS",IF(F32=17,"DIECISIETE",IF(F32=18,"DIECIOCHO", IF(F32=19,"DIECINUEVE",IF(F32=20,"VEINTE",ERROR))))))))))</f>
+        <v>ONCE</v>
+      </c>
+      <c r="H32" s="4">
+        <v>4</v>
+      </c>
+      <c r="I32" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J32" s="19"/>
       <c r="M32" s="9"/>
-      <c r="N32" s="41"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="11"/>
+      <c r="N32" s="43">
+        <v>20171</v>
+      </c>
+      <c r="O32" s="4">
+        <v>21</v>
+      </c>
+      <c r="P32" s="11" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="33" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19"/>
-      <c r="B33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="9"/>
+      <c r="D33" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="E33" s="9"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="38"/>
+      <c r="F33" s="57">
+        <v>12</v>
+      </c>
+      <c r="G33" s="4" t="str">
+        <f>IF(F33=11,"ONCE",IF(F33=12,"DOCE",IF(F33=13,"TRECE",IF(F33=14,"CATORCE",IF(F33=15,"QUINCE",IF(F33=16,"DIECISEIS",IF(F33=17,"DIECISIETE",IF(F33=18,"DIECIOCHO", IF(F33=19,"DIECINUEVE",IF(F33=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="H33" s="4">
+        <v>3</v>
+      </c>
+      <c r="I33" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J33" s="19"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="41"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="11"/>
-    </row>
-    <row r="34" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N33" s="43">
+        <v>20162</v>
+      </c>
+      <c r="O33" s="4">
+        <v>21</v>
+      </c>
+      <c r="P33" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
       <c r="B34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
+        <v>61</v>
+      </c>
+      <c r="C34" s="40"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="38" t="str">
+      <c r="I34" s="40" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J34" s="19"/>
       <c r="M34" s="5" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="N34" s="19"/>
       <c r="O34" s="4"/>
@@ -1962,118 +2729,235 @@
     </row>
     <row r="35" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19"/>
-      <c r="B35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="9"/>
+      <c r="D35" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E35" s="9"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="38"/>
+      <c r="F35" s="57">
+        <v>16</v>
+      </c>
+      <c r="G35" s="4" t="str">
+        <f>IF(F35=11,"ONCE",IF(F35=12,"DOCE",IF(F35=13,"TRECE",IF(F35=14,"CATORCE",IF(F35=15,"QUINCE",IF(F35=16,"DIECISEIS",IF(F35=17,"DIECISIETE",IF(F35=18,"DIECIOCHO", IF(F35=19,"DIECINUEVE",IF(F35=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISEIS</v>
+      </c>
+      <c r="H35" s="4">
+        <v>4</v>
+      </c>
+      <c r="I35" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J35" s="19"/>
       <c r="M35" s="9"/>
-      <c r="N35" s="41"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="11"/>
+      <c r="N35" s="43">
+        <v>20172</v>
+      </c>
+      <c r="O35" s="4">
+        <v>21</v>
+      </c>
+      <c r="P35" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="36" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
-      <c r="B36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="9"/>
+      <c r="D36" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="E36" s="9"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="38"/>
+      <c r="F36" s="57">
+        <v>12</v>
+      </c>
+      <c r="G36" s="4" t="str">
+        <f>IF(F36=11,"ONCE",IF(F36=12,"DOCE",IF(F36=13,"TRECE",IF(F36=14,"CATORCE",IF(F36=15,"QUINCE",IF(F36=16,"DIECISEIS",IF(F36=17,"DIECISIETE",IF(F36=18,"DIECIOCHO", IF(F36=19,"DIECINUEVE",IF(F36=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="H36" s="4">
+        <v>3</v>
+      </c>
+      <c r="I36" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J36" s="19"/>
       <c r="M36" s="9"/>
-      <c r="N36" s="41"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="11"/>
+      <c r="N36" s="43">
+        <v>20172</v>
+      </c>
+      <c r="O36" s="4">
+        <v>21</v>
+      </c>
+      <c r="P36" s="11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="37" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
-      <c r="B37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="9"/>
+      <c r="D37" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="E37" s="9"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="38"/>
+      <c r="F37" s="57">
+        <v>13</v>
+      </c>
+      <c r="G37" s="4" t="str">
+        <f>IF(F37=11,"ONCE",IF(F37=12,"DOCE",IF(F37=13,"TRECE",IF(F37=14,"CATORCE",IF(F37=15,"QUINCE",IF(F37=16,"DIECISEIS",IF(F37=17,"DIECISIETE",IF(F37=18,"DIECIOCHO", IF(F37=19,"DIECINUEVE",IF(F37=20,"VEINTE",ERROR))))))))))</f>
+        <v>TRECE</v>
+      </c>
+      <c r="H37" s="4">
+        <v>3</v>
+      </c>
+      <c r="I37" s="40" t="str">
+        <f t="shared" ref="I37:I47" si="1">+CONCATENATE(N37,O37,P37)</f>
+        <v>2021221021</v>
+      </c>
       <c r="J37" s="19"/>
       <c r="M37" s="9"/>
-      <c r="N37" s="41"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="11"/>
+      <c r="N37" s="43">
+        <v>20212</v>
+      </c>
+      <c r="O37" s="4">
+        <v>21</v>
+      </c>
+      <c r="P37" s="11" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="38" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
-      <c r="B38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="C38" s="4"/>
-      <c r="D38" s="9"/>
+      <c r="D38" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="E38" s="9"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="38"/>
+      <c r="F38" s="57">
+        <v>15</v>
+      </c>
+      <c r="G38" s="4" t="str">
+        <f>IF(F38=11,"ONCE",IF(F38=12,"DOCE",IF(F38=13,"TRECE",IF(F38=14,"CATORCE",IF(F38=15,"QUINCE",IF(F38=16,"DIECISEIS",IF(F38=17,"DIECISIETE",IF(F38=18,"DIECIOCHO", IF(F38=19,"DIECINUEVE",IF(F38=20,"VEINTE",ERROR))))))))))</f>
+        <v>QUINCE</v>
+      </c>
+      <c r="H38" s="4">
+        <v>5</v>
+      </c>
+      <c r="I38" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J38" s="19"/>
       <c r="M38" s="9"/>
-      <c r="N38" s="41"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="11"/>
+      <c r="N38" s="43">
+        <v>20172</v>
+      </c>
+      <c r="O38" s="4">
+        <v>21</v>
+      </c>
+      <c r="P38" s="11" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="39" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="19"/>
-      <c r="B39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="9"/>
+      <c r="D39" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="E39" s="9"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="38"/>
+      <c r="F39" s="57">
+        <v>16</v>
+      </c>
+      <c r="G39" s="4" t="str">
+        <f>IF(F39=11,"ONCE",IF(F39=12,"DOCE",IF(F39=13,"TRECE",IF(F39=14,"CATORCE",IF(F39=15,"QUINCE",IF(F39=16,"DIECISEIS",IF(F39=17,"DIECISIETE",IF(F39=18,"DIECIOCHO", IF(F39=19,"DIECINUEVE",IF(F39=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISEIS</v>
+      </c>
+      <c r="H39" s="4">
+        <v>6</v>
+      </c>
+      <c r="I39" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>2021221023</v>
+      </c>
       <c r="J39" s="19"/>
       <c r="M39" s="9"/>
-      <c r="N39" s="41"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="11"/>
+      <c r="N39" s="43">
+        <v>20212</v>
+      </c>
+      <c r="O39" s="4">
+        <v>21</v>
+      </c>
+      <c r="P39" s="11" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="40" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="19"/>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="C40" s="4"/>
-      <c r="D40" s="9"/>
+      <c r="D40" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="E40" s="9"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="38"/>
+      <c r="F40" s="57">
+        <v>13</v>
+      </c>
+      <c r="G40" s="4" t="str">
+        <f>IF(F40=11,"ONCE",IF(F40=12,"DOCE",IF(F40=13,"TRECE",IF(F40=14,"CATORCE",IF(F40=15,"QUINCE",IF(F40=16,"DIECISEIS",IF(F40=17,"DIECISIETE",IF(F40=18,"DIECIOCHO", IF(F40=19,"DIECINUEVE",IF(F40=20,"VEINTE",ERROR))))))))))</f>
+        <v>TRECE</v>
+      </c>
+      <c r="H40" s="4">
+        <v>3</v>
+      </c>
+      <c r="I40" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>2021121024</v>
+      </c>
       <c r="J40" s="19"/>
       <c r="M40" s="9"/>
-      <c r="N40" s="41"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="11"/>
+      <c r="N40" s="43">
+        <v>20211</v>
+      </c>
+      <c r="O40" s="4">
+        <v>21</v>
+      </c>
+      <c r="P40" s="11" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="41" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19"/>
       <c r="B41" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="38"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
+        <v>80</v>
+      </c>
+      <c r="C41" s="40"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="38" t="str">
-        <f t="shared" ref="I37:I47" si="1">+CONCATENATE(N41,O41,P41)</f>
+      <c r="I41" s="40" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J41" s="19"/>
       <c r="M41" s="5" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="N41" s="19"/>
       <c r="O41" s="4"/>
@@ -2081,106 +2965,224 @@
     </row>
     <row r="42" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
-      <c r="B42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="C42" s="4"/>
-      <c r="D42" s="9"/>
+      <c r="D42" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="E42" s="9"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="38"/>
+      <c r="F42" s="57">
+        <v>12</v>
+      </c>
+      <c r="G42" s="4" t="str">
+        <f>IF(F42=11,"ONCE",IF(F42=12,"DOCE",IF(F42=13,"TRECE",IF(F42=14,"CATORCE",IF(F42=15,"QUINCE",IF(F42=16,"DIECISEIS",IF(F42=17,"DIECISIETE",IF(F42=18,"DIECIOCHO", IF(F42=19,"DIECINUEVE",IF(F42=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="H42" s="4">
+        <v>3</v>
+      </c>
+      <c r="I42" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J42" s="19"/>
       <c r="M42" s="9"/>
-      <c r="N42" s="41"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="11"/>
+      <c r="N42" s="43">
+        <v>20191</v>
+      </c>
+      <c r="O42" s="4">
+        <v>21</v>
+      </c>
+      <c r="P42" s="11" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="43" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19"/>
-      <c r="B43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="C43" s="4"/>
-      <c r="D43" s="9"/>
+      <c r="D43" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="E43" s="9"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="38"/>
+      <c r="F43" s="57">
+        <v>18</v>
+      </c>
+      <c r="G43" s="4" t="str">
+        <f>IF(F43=11,"ONCE",IF(F43=12,"DOCE",IF(F43=13,"TRECE",IF(F43=14,"CATORCE",IF(F43=15,"QUINCE",IF(F43=16,"DIECISEIS",IF(F43=17,"DIECISIETE",IF(F43=18,"DIECIOCHO", IF(F43=19,"DIECINUEVE",IF(F43=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECIOCHO</v>
+      </c>
+      <c r="H43" s="4">
+        <v>3</v>
+      </c>
+      <c r="I43" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>2021221026</v>
+      </c>
       <c r="J43" s="19"/>
       <c r="M43" s="9"/>
-      <c r="N43" s="41"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="11"/>
+      <c r="N43" s="43">
+        <v>20212</v>
+      </c>
+      <c r="O43" s="4">
+        <v>21</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="44" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19"/>
-      <c r="B44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="C44" s="4"/>
-      <c r="D44" s="9"/>
+      <c r="D44" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="E44" s="9"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="38"/>
+      <c r="F44" s="57">
+        <v>11</v>
+      </c>
+      <c r="G44" s="4" t="str">
+        <f>IF(F44=11,"ONCE",IF(F44=12,"DOCE",IF(F44=13,"TRECE",IF(F44=14,"CATORCE",IF(F44=15,"QUINCE",IF(F44=16,"DIECISEIS",IF(F44=17,"DIECISIETE",IF(F44=18,"DIECIOCHO", IF(F44=19,"DIECINUEVE",IF(F44=20,"VEINTE",ERROR))))))))))</f>
+        <v>ONCE</v>
+      </c>
+      <c r="H44" s="4">
+        <v>4</v>
+      </c>
+      <c r="I44" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>2021221027</v>
+      </c>
       <c r="J44" s="19"/>
       <c r="M44" s="9"/>
-      <c r="N44" s="41"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="11"/>
+      <c r="N44" s="43">
+        <v>20212</v>
+      </c>
+      <c r="O44" s="4">
+        <v>21</v>
+      </c>
+      <c r="P44" s="11" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="45" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="19"/>
-      <c r="B45" s="4"/>
+      <c r="B45" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="9"/>
+      <c r="D45" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="E45" s="9"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="38"/>
+      <c r="F45" s="57">
+        <v>12</v>
+      </c>
+      <c r="G45" s="4" t="str">
+        <f>IF(F45=11,"ONCE",IF(F45=12,"DOCE",IF(F45=13,"TRECE",IF(F45=14,"CATORCE",IF(F45=15,"QUINCE",IF(F45=16,"DIECISEIS",IF(F45=17,"DIECISIETE",IF(F45=18,"DIECIOCHO", IF(F45=19,"DIECINUEVE",IF(F45=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="H45" s="4">
+        <v>3</v>
+      </c>
+      <c r="I45" s="40" t="s">
+        <v>6</v>
+      </c>
       <c r="J45" s="19"/>
       <c r="M45" s="9"/>
-      <c r="N45" s="41"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="11"/>
+      <c r="N45" s="43">
+        <v>20191</v>
+      </c>
+      <c r="O45" s="4">
+        <v>21</v>
+      </c>
+      <c r="P45" s="11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="46" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
-      <c r="B46" s="4"/>
+      <c r="B46" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="C46" s="4"/>
-      <c r="D46" s="9"/>
+      <c r="D46" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="E46" s="9"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="38"/>
+      <c r="F46" s="57">
+        <v>11</v>
+      </c>
+      <c r="G46" s="4" t="str">
+        <f>IF(F46=11,"ONCE",IF(F46=12,"DOCE",IF(F46=13,"TRECE",IF(F46=14,"CATORCE",IF(F46=15,"QUINCE",IF(F46=16,"DIECISEIS",IF(F46=17,"DIECISIETE",IF(F46=18,"DIECIOCHO", IF(F46=19,"DIECINUEVE",IF(F46=20,"VEINTE",ERROR))))))))))</f>
+        <v>ONCE</v>
+      </c>
+      <c r="H46" s="4">
+        <v>6</v>
+      </c>
+      <c r="I46" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>2021121029</v>
+      </c>
       <c r="J46" s="19"/>
       <c r="M46" s="9"/>
-      <c r="N46" s="41"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="11"/>
+      <c r="N46" s="43">
+        <v>20211</v>
+      </c>
+      <c r="O46" s="4">
+        <v>21</v>
+      </c>
+      <c r="P46" s="11" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="47" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
-      <c r="B47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="9"/>
+      <c r="D47" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="E47" s="9"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="38"/>
+      <c r="F47" s="57">
+        <v>16</v>
+      </c>
+      <c r="G47" s="4" t="str">
+        <f>IF(F47=11,"ONCE",IF(F47=12,"DOCE",IF(F47=13,"TRECE",IF(F47=14,"CATORCE",IF(F47=15,"QUINCE",IF(F47=16,"DIECISEIS",IF(F47=17,"DIECISIETE",IF(F47=18,"DIECIOCHO", IF(F47=19,"DIECINUEVE",IF(F47=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISEIS</v>
+      </c>
+      <c r="H47" s="4">
+        <v>3</v>
+      </c>
+      <c r="I47" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>2022121030</v>
+      </c>
       <c r="J47" s="19"/>
       <c r="M47" s="9"/>
-      <c r="N47" s="41"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="11"/>
+      <c r="N47" s="43">
+        <v>20221</v>
+      </c>
+      <c r="O47" s="4">
+        <v>21</v>
+      </c>
+      <c r="P47" s="11" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="48" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
       <c r="B48" s="20"/>
       <c r="C48" s="17"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
       <c r="F48" s="17"/>
       <c r="G48" s="15"/>
       <c r="H48" s="22"/>
@@ -2273,17 +3275,17 @@
   </sheetPr>
   <dimension ref="B1:S51"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="28" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" style="28" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="60" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="60" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="21" customWidth="1"/>
     <col min="6" max="6" width="3.42578125" style="23" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="23" customWidth="1"/>
     <col min="8" max="8" width="1.140625" style="19" customWidth="1"/>
@@ -2301,493 +3303,921 @@
     <row r="1" spans="2:19" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="20"/>
       <c r="C1" s="26"/>
-      <c r="E1" s="61"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="22"/>
       <c r="P1" s="27" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="Q1" s="16"/>
       <c r="R1" s="14" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="38"/>
+        <v>102</v>
+      </c>
+      <c r="C2" s="51"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="40"/>
       <c r="G2" s="1"/>
       <c r="K2" s="29" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="L2" s="29"/>
       <c r="M2" s="21"/>
       <c r="N2" s="30"/>
       <c r="P2" s="27" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="Q2" s="16"/>
       <c r="R2" s="14" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="S2" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="56"/>
+      <c r="E3" s="4" t="str">
+        <f>IF(D3=11,"ONCE",IF(D3=12,"DOCE",IF(D3=13,"TRECE",IF(D3=14,"CATORCE",IF(D3=15,"QUINCE",IF(D3=16,"DIECISEIS",IF(D3=17,"DIECISIETE",IF(D3=18,"DIECIOCHO", IF(D3=19,"DIECINUEVE",IF(D3=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="F3" s="59">
+        <v>2</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>6</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="14"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
+      <c r="L3" s="43">
+        <v>20192</v>
+      </c>
+      <c r="M3" s="15">
+        <v>21</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>108</v>
+      </c>
       <c r="P3" s="27" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="Q3" s="16"/>
       <c r="R3" s="14" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="56"/>
+      <c r="B4" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="4">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <f>IF(D4=11,"ONCE",IF(D4=12,"DOCE",IF(D4=13,"TRECE",IF(D4=14,"CATORCE",IF(D4=15,"QUINCE",IF(D4=16,"DIECISEIS",IF(D4=17,"DIECISIETE",IF(D4=18,"DIECIOCHO", IF(D4=19,"DIECINUEVE",IF(D4=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="F4" s="59">
+        <v>4</v>
+      </c>
+      <c r="G4" s="58" t="str">
+        <f t="shared" ref="G4:G23" si="0">+CONCATENATE(L4,M4,N4)</f>
+        <v>2022121032</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="14"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="16"/>
+      <c r="L4" s="43">
+        <v>20221</v>
+      </c>
+      <c r="M4" s="15">
+        <v>21</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>114</v>
+      </c>
       <c r="P4" s="27" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="Q4" s="16"/>
       <c r="R4" s="14" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="S4" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="4">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="56"/>
+      <c r="E5" s="4" t="str">
+        <f>IF(D5=11,"ONCE",IF(D5=12,"DOCE",IF(D5=13,"TRECE",IF(D5=14,"CATORCE",IF(D5=15,"QUINCE",IF(D5=16,"DIECISEIS",IF(D5=17,"DIECISIETE",IF(D5=18,"DIECIOCHO", IF(D5=19,"DIECINUEVE",IF(D5=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECIOCHO</v>
+      </c>
+      <c r="F5" s="59">
+        <v>4</v>
+      </c>
+      <c r="G5" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022121033</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="16"/>
+      <c r="L5" s="43">
+        <v>20221</v>
+      </c>
+      <c r="M5" s="15">
+        <v>21</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="P5" s="27" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="Q5" s="16"/>
       <c r="R5" s="14" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="56"/>
+      <c r="B6" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="4">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="str">
+        <f>IF(D6=11,"ONCE",IF(D6=12,"DOCE",IF(D6=13,"TRECE",IF(D6=14,"CATORCE",IF(D6=15,"QUINCE",IF(D6=16,"DIECISEIS",IF(D6=17,"DIECISIETE",IF(D6=18,"DIECIOCHO", IF(D6=19,"DIECINUEVE",IF(D6=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="F6" s="59">
+        <v>2</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>6</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="14"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="16"/>
+      <c r="L6" s="43">
+        <v>20192</v>
+      </c>
+      <c r="M6" s="15">
+        <v>21</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>126</v>
+      </c>
       <c r="P6" s="27" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="Q6" s="16"/>
       <c r="R6" s="14" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="56"/>
+      <c r="B7" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="4">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4" t="str">
+        <f>IF(D7=11,"ONCE",IF(D7=12,"DOCE",IF(D7=13,"TRECE",IF(D7=14,"CATORCE",IF(D7=15,"QUINCE",IF(D7=16,"DIECISEIS",IF(D7=17,"DIECISIETE",IF(D7=18,"DIECIOCHO", IF(D7=19,"DIECINUEVE",IF(D7=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="F7" s="59">
+        <v>6</v>
+      </c>
+      <c r="G7" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2021221035</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="16"/>
+      <c r="L7" s="43">
+        <v>20212</v>
+      </c>
+      <c r="M7" s="15">
+        <v>21</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="8" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="50"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="56"/>
+      <c r="B8" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="4">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="str">
+        <f>IF(D8=11,"ONCE",IF(D8=12,"DOCE",IF(D8=13,"TRECE",IF(D8=14,"CATORCE",IF(D8=15,"QUINCE",IF(D8=16,"DIECISEIS",IF(D8=17,"DIECISIETE",IF(D8=18,"DIECIOCHO", IF(D8=19,"DIECINUEVE",IF(D8=20,"VEINTE",ERROR))))))))))</f>
+        <v>ONCE</v>
+      </c>
+      <c r="F8" s="59">
+        <v>2</v>
+      </c>
+      <c r="G8" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2021121051</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="16"/>
+      <c r="L8" s="43">
+        <v>20211</v>
+      </c>
+      <c r="M8" s="15">
+        <v>21</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="9" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="56" t="str">
-        <f t="shared" ref="G4:G23" si="0">+CONCATENATE(L9,M9,N9)</f>
+        <v>133</v>
+      </c>
+      <c r="C9" s="53"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="58" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="39"/>
+      <c r="K9" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="L9" s="41"/>
       <c r="M9" s="15"/>
       <c r="N9" s="30"/>
     </row>
     <row r="10" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="50"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="56"/>
+      <c r="B10" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="4">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="str">
+        <f>IF(D10=11,"ONCE",IF(D10=12,"DOCE",IF(D10=13,"TRECE",IF(D10=14,"CATORCE",IF(D10=15,"QUINCE",IF(D10=16,"DIECISEIS",IF(D10=17,"DIECISIETE",IF(D10=18,"DIECIOCHO", IF(D10=19,"DIECINUEVE",IF(D10=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="F10" s="59">
+        <v>4</v>
+      </c>
+      <c r="G10" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022121036</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="16"/>
+      <c r="L10" s="43">
+        <v>20221</v>
+      </c>
+      <c r="M10" s="15">
+        <v>21</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="11" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="56"/>
+      <c r="B11" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="4">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4" t="str">
+        <f>IF(D11=11,"ONCE",IF(D11=12,"DOCE",IF(D11=13,"TRECE",IF(D11=14,"CATORCE",IF(D11=15,"QUINCE",IF(D11=16,"DIECISEIS",IF(D11=17,"DIECISIETE",IF(D11=18,"DIECIOCHO", IF(D11=19,"DIECINUEVE",IF(D11=20,"VEINTE",ERROR))))))))))</f>
+        <v>ONCE</v>
+      </c>
+      <c r="F11" s="59">
+        <v>3</v>
+      </c>
+      <c r="G11" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2021121037</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
+      <c r="L11" s="43">
+        <v>20211</v>
+      </c>
+      <c r="M11" s="15">
+        <v>21</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="56"/>
+      <c r="B12" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="4">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="str">
+        <f>IF(D12=11,"ONCE",IF(D12=12,"DOCE",IF(D12=13,"TRECE",IF(D12=14,"CATORCE",IF(D12=15,"QUINCE",IF(D12=16,"DIECISEIS",IF(D12=17,"DIECISIETE",IF(D12=18,"DIECIOCHO", IF(D12=19,"DIECINUEVE",IF(D12=20,"VEINTE",ERROR))))))))))</f>
+        <v>DOCE</v>
+      </c>
+      <c r="F12" s="59">
+        <v>3</v>
+      </c>
+      <c r="G12" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022221038</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="14"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="16"/>
+      <c r="L12" s="43">
+        <v>20222</v>
+      </c>
+      <c r="M12" s="15">
+        <v>21</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="13" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="56"/>
+      <c r="B13" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="4">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4" t="str">
+        <f>IF(D13=11,"ONCE",IF(D13=12,"DOCE",IF(D13=13,"TRECE",IF(D13=14,"CATORCE",IF(D13=15,"QUINCE",IF(D13=16,"DIECISEIS",IF(D13=17,"DIECISIETE",IF(D13=18,"DIECIOCHO", IF(D13=19,"DIECINUEVE",IF(D13=20,"VEINTE",ERROR))))))))))</f>
+        <v>QUINCE</v>
+      </c>
+      <c r="F13" s="59">
+        <v>6</v>
+      </c>
+      <c r="G13" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2021121039</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="16"/>
+      <c r="L13" s="43">
+        <v>20211</v>
+      </c>
+      <c r="M13" s="15">
+        <v>21</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="14" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="56"/>
+      <c r="B14" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="4">
+        <v>16</v>
+      </c>
+      <c r="E14" s="4" t="str">
+        <f>IF(D14=11,"ONCE",IF(D14=12,"DOCE",IF(D14=13,"TRECE",IF(D14=14,"CATORCE",IF(D14=15,"QUINCE",IF(D14=16,"DIECISEIS",IF(D14=17,"DIECISIETE",IF(D14=18,"DIECIOCHO", IF(D14=19,"DIECINUEVE",IF(D14=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISEIS</v>
+      </c>
+      <c r="F14" s="59">
+        <v>3</v>
+      </c>
+      <c r="G14" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022121040</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="16"/>
+      <c r="L14" s="43">
+        <v>20221</v>
+      </c>
+      <c r="M14" s="15">
+        <v>21</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="15" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="50"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="56"/>
+      <c r="B15" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="4">
+        <v>17</v>
+      </c>
+      <c r="E15" s="4" t="str">
+        <f>IF(D15=11,"ONCE",IF(D15=12,"DOCE",IF(D15=13,"TRECE",IF(D15=14,"CATORCE",IF(D15=15,"QUINCE",IF(D15=16,"DIECISEIS",IF(D15=17,"DIECISIETE",IF(D15=18,"DIECIOCHO", IF(D15=19,"DIECINUEVE",IF(D15=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="F15" s="59">
+        <v>2</v>
+      </c>
+      <c r="G15" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022121052</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="16"/>
+      <c r="L15" s="43">
+        <v>20221</v>
+      </c>
+      <c r="M15" s="15">
+        <v>21</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="56" t="str">
+        <v>149</v>
+      </c>
+      <c r="C16" s="53"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="58" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="L16" s="39"/>
+      <c r="K16" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="L16" s="41"/>
       <c r="M16" s="15"/>
       <c r="N16" s="30"/>
     </row>
     <row r="17" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="56"/>
+      <c r="B17" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="4">
+        <v>17</v>
+      </c>
+      <c r="E17" s="4" t="str">
+        <f>IF(D17=11,"ONCE",IF(D17=12,"DOCE",IF(D17=13,"TRECE",IF(D17=14,"CATORCE",IF(D17=15,"QUINCE",IF(D17=16,"DIECISEIS",IF(D17=17,"DIECISIETE",IF(D17=18,"DIECIOCHO", IF(D17=19,"DIECINUEVE",IF(D17=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="F17" s="59">
+        <v>3</v>
+      </c>
+      <c r="G17" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022221041</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="16"/>
+      <c r="L17" s="15">
+        <v>20222</v>
+      </c>
+      <c r="M17" s="15">
+        <v>21</v>
+      </c>
+      <c r="N17" s="16" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="18" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="56"/>
+      <c r="B18" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="4">
+        <v>15</v>
+      </c>
+      <c r="E18" s="4" t="str">
+        <f>IF(D18=11,"ONCE",IF(D18=12,"DOCE",IF(D18=13,"TRECE",IF(D18=14,"CATORCE",IF(D18=15,"QUINCE",IF(D18=16,"DIECISEIS",IF(D18=17,"DIECISIETE",IF(D18=18,"DIECIOCHO", IF(D18=19,"DIECINUEVE",IF(D18=20,"VEINTE",ERROR))))))))))</f>
+        <v>QUINCE</v>
+      </c>
+      <c r="F18" s="59">
+        <v>4</v>
+      </c>
+      <c r="G18" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022221042</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="16"/>
+      <c r="L18" s="15">
+        <v>20222</v>
+      </c>
+      <c r="M18" s="15">
+        <v>21</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="19" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="56"/>
+      <c r="B19" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="4">
+        <v>18</v>
+      </c>
+      <c r="E19" s="4" t="str">
+        <f>IF(D19=11,"ONCE",IF(D19=12,"DOCE",IF(D19=13,"TRECE",IF(D19=14,"CATORCE",IF(D19=15,"QUINCE",IF(D19=16,"DIECISEIS",IF(D19=17,"DIECISIETE",IF(D19=18,"DIECIOCHO", IF(D19=19,"DIECINUEVE",IF(D19=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECIOCHO</v>
+      </c>
+      <c r="F19" s="59">
+        <v>10</v>
+      </c>
+      <c r="G19" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022221043</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="16"/>
+      <c r="L19" s="15">
+        <v>20222</v>
+      </c>
+      <c r="M19" s="15">
+        <v>21</v>
+      </c>
+      <c r="N19" s="16" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="20" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="56"/>
+      <c r="B20" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="4">
+        <v>18</v>
+      </c>
+      <c r="E20" s="4" t="str">
+        <f>IF(D20=11,"ONCE",IF(D20=12,"DOCE",IF(D20=13,"TRECE",IF(D20=14,"CATORCE",IF(D20=15,"QUINCE",IF(D20=16,"DIECISEIS",IF(D20=17,"DIECISIETE",IF(D20=18,"DIECIOCHO", IF(D20=19,"DIECINUEVE",IF(D20=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECIOCHO</v>
+      </c>
+      <c r="F20" s="59">
+        <v>3</v>
+      </c>
+      <c r="G20" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022221044</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="16"/>
+      <c r="L20" s="15">
+        <v>20222</v>
+      </c>
+      <c r="M20" s="15">
+        <v>21</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="21" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="50"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="56"/>
+      <c r="B21" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="4">
+        <v>17</v>
+      </c>
+      <c r="E21" s="4" t="str">
+        <f>IF(D21=11,"ONCE",IF(D21=12,"DOCE",IF(D21=13,"TRECE",IF(D21=14,"CATORCE",IF(D21=15,"QUINCE",IF(D21=16,"DIECISEIS",IF(D21=17,"DIECISIETE",IF(D21=18,"DIECIOCHO", IF(D21=19,"DIECINUEVE",IF(D21=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="F21" s="59">
+        <v>2</v>
+      </c>
+      <c r="G21" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2022121054</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="14"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="16"/>
+      <c r="L21" s="15">
+        <v>20221</v>
+      </c>
+      <c r="M21" s="15">
+        <v>21</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="22" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="65"/>
+      <c r="B22" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="38" t="str">
+      <c r="G22" s="40" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="39" t="s">
-        <v>27</v>
+      <c r="K22" s="41" t="s">
+        <v>162</v>
       </c>
       <c r="L22" s="14"/>
       <c r="M22" s="15"/>
       <c r="N22" s="18"/>
     </row>
     <row r="23" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="50"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="56"/>
+      <c r="B23" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="4">
+        <v>16</v>
+      </c>
+      <c r="E23" s="4" t="str">
+        <f>IF(D23=11,"ONCE",IF(D23=12,"DOCE",IF(D23=13,"TRECE",IF(D23=14,"CATORCE",IF(D23=15,"QUINCE",IF(D23=16,"DIECISEIS",IF(D23=17,"DIECISIETE",IF(D23=18,"DIECIOCHO", IF(D23=19,"DIECINUEVE",IF(D23=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISEIS</v>
+      </c>
+      <c r="F23" s="4">
+        <v>6</v>
+      </c>
+      <c r="G23" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>2023121045</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="16"/>
+      <c r="J23" s="2" t="str">
+        <f t="shared" ref="J23:K24" si="1">+CONCATENATE(O23,P23,Q23)</f>
+        <v/>
+      </c>
+      <c r="K23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L23" s="15">
+        <v>20231</v>
+      </c>
+      <c r="M23" s="15">
+        <v>21</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="24" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="56"/>
+      <c r="B24" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="4">
+        <v>17</v>
+      </c>
+      <c r="E24" s="4" t="str">
+        <f>IF(D24=11,"ONCE",IF(D24=12,"DOCE",IF(D24=13,"TRECE",IF(D24=14,"CATORCE",IF(D24=15,"QUINCE",IF(D24=16,"DIECISEIS",IF(D24=17,"DIECISIETE",IF(D24=18,"DIECIOCHO", IF(D24=19,"DIECINUEVE",IF(D24=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="F24" s="4">
+        <v>15</v>
+      </c>
+      <c r="G24" s="58" t="str">
+        <f t="shared" ref="G24:G27" si="2">+CONCATENATE(L24,M24,N24)</f>
+        <v>2023121046</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="16"/>
+      <c r="J24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L24" s="15">
+        <v>20231</v>
+      </c>
+      <c r="M24" s="15">
+        <v>21</v>
+      </c>
+      <c r="N24" s="16" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="25" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="65"/>
+      <c r="B25" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="52"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="56" t="str">
-        <f t="shared" ref="G24:G27" si="1">+CONCATENATE(L25,M25,N25)</f>
+      <c r="G25" s="58" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="40" t="s">
-        <v>28</v>
+      <c r="K25" s="42" t="s">
+        <v>167</v>
       </c>
       <c r="L25" s="9"/>
       <c r="M25" s="15"/>
       <c r="N25" s="18"/>
     </row>
     <row r="26" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="56"/>
+      <c r="B26" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" s="53" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="e">
+        <f>IF(D26=11,"ONCE",IF(D26=12,"DOCE",IF(D26=13,"TRECE",IF(D26=14,"CATORCE",IF(D26=15,"QUINCE",IF(D26=16,"DIECISEIS",IF(D26=17,"DIECISIETE",IF(D26=18,"DIECIOCHO", IF(D26=19,"DIECINUEVE",IF(D26=20,"VEINTE",ERROR))))))))))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F26" s="4">
+        <v>6</v>
+      </c>
+      <c r="G26" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v>2023221047</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="14"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="16"/>
+      <c r="L26" s="15">
+        <v>20232</v>
+      </c>
+      <c r="M26" s="15">
+        <v>21</v>
+      </c>
+      <c r="N26" s="16" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="27" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="56"/>
+      <c r="B27" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="4">
+        <v>17</v>
+      </c>
+      <c r="E27" s="4" t="str">
+        <f>IF(D27=11,"ONCE",IF(D27=12,"DOCE",IF(D27=13,"TRECE",IF(D27=14,"CATORCE",IF(D27=15,"QUINCE",IF(D27=16,"DIECISEIS",IF(D27=17,"DIECISIETE",IF(D27=18,"DIECIOCHO", IF(D27=19,"DIECINUEVE",IF(D27=20,"VEINTE",ERROR))))))))))</f>
+        <v>DIECISIETE</v>
+      </c>
+      <c r="F27" s="4">
+        <v>15</v>
+      </c>
+      <c r="G27" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v>2023221048</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="16"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="15">
+        <v>20232</v>
+      </c>
+      <c r="M27" s="15">
+        <v>21</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="28" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="14"/>
@@ -2809,8 +4239,8 @@
     <row r="30" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="27"/>
       <c r="C30" s="27"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="14"/>
@@ -2827,8 +4257,8 @@
     <row r="31" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="14"/>
@@ -2845,8 +4275,8 @@
     <row r="32" spans="2:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="14"/>
@@ -2861,8 +4291,8 @@
       <c r="Q32" s="14"/>
     </row>
     <row r="33" spans="2:17" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
       <c r="H33" s="14"/>
@@ -2879,92 +4309,92 @@
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="31"/>
       <c r="C34" s="32"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="68"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="19"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="31"/>
       <c r="C35" s="32"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="68"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="19"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="D36" s="67"/>
-      <c r="E36" s="68"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="D37" s="67"/>
-      <c r="E37" s="68"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="19"/>
     </row>
     <row r="38" spans="2:17" s="34" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B38" s="33"/>
       <c r="C38" s="33"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="66"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="14"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
       <c r="H38" s="14"/>
-      <c r="N38" s="35"/>
+      <c r="N38" s="36"/>
       <c r="P38" s="25"/>
     </row>
     <row r="39" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="37"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="71"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C45" s="37"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="68"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="71"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3018,23 +4448,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8e5d010b-d12e-47a7-8051-5298d0c42759" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010007E5F67EA1DF3641A73DB9BA813317B7" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f72d9bff1373ddf58a359e5fcd415a6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e5d010b-d12e-47a7-8051-5298d0c42759" xmlns:ns4="ea131169-3452-48c5-b768-60ccd9d6662b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58659ac67a12a69fb5965e0685f988f4" ns3:_="" ns4:_="">
     <xsd:import namespace="8e5d010b-d12e-47a7-8051-5298d0c42759"/>
@@ -3273,10 +4686,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8e5d010b-d12e-47a7-8051-5298d0c42759" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3C9C25C-43E4-4613-98E4-9C1DBCB0F7AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{174D919E-B1B1-4D50-8A19-E2217CCEB65D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8e5d010b-d12e-47a7-8051-5298d0c42759"/>
+    <ds:schemaRef ds:uri="ea131169-3452-48c5-b768-60ccd9d6662b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3299,20 +4740,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{174D919E-B1B1-4D50-8A19-E2217CCEB65D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3C9C25C-43E4-4613-98E4-9C1DBCB0F7AE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8e5d010b-d12e-47a7-8051-5298d0c42759"/>
-    <ds:schemaRef ds:uri="ea131169-3452-48c5-b768-60ccd9d6662b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>